<commit_message>
Adding analyzers and testing results
</commit_message>
<xml_diff>
--- a/misc analysis/Results analysis (Annual Data).xlsx
+++ b/misc analysis/Results analysis (Annual Data).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fega\Desktop\portfolio-allocation\misc analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C69128-4B43-4641-BA81-176155F92BFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CC1170-4524-4052-B1AB-58D908275DFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{161C5C75-020D-46B4-9A37-BBAEE0A65B1A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="57">
   <si>
     <t>DATE</t>
   </si>
@@ -174,34 +174,53 @@
     <t>initial money 1m (fund true, no monthly)</t>
   </si>
   <si>
-    <t>rtot</t>
-  </si>
-  <si>
-    <t>ravg</t>
-  </si>
-  <si>
-    <t>rnorm</t>
-  </si>
-  <si>
-    <t>rnorm100</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
     <t>drowdown</t>
+  </si>
+  <si>
+    <t>OrderedDict([(datetime.datetime(2019, 2, 7, 0, 0), -0.009399013896574016),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             (datetime.datetime(2019, 2, 8, 0, 0), 0.0006758152048207056),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             (datetime.datetime(2019, 2, 11, 0, 0), 0.0007086868909718171),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             (datetime.datetime(2019, 2, 12, 0, 0), 0.012804893098913972),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             (datetime.datetime(2019, 2, 13, 0, 0), 0.0030187394455014303),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             (datetime.datetime(2019, 2, 14, 0, 0), -0.0026545548555742225),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             (datetime.datetime(2019, 2, 15, 0, 0), 0.010817534992512602),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             (datetime.datetime(2019, 2, 18, 0, 0), 0.0),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             (datetime.datetime(2019, 2, 19, 0, 0), 0.0014972815135696387)])</t>
+  </si>
+  <si>
+    <t>SR (r=1%) logret</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="167" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -327,7 +346,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -372,9 +391,12 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="3" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -4567,8 +4589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB9A6555-6A22-46D7-BF58-F136DBB594A7}">
   <dimension ref="A1:AR55"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5941,7 +5963,7 @@
   <dimension ref="A3:R48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5951,7 +5973,7 @@
     <col min="3" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6643,20 +6665,52 @@
       <c r="H18" t="s">
         <v>38</v>
       </c>
+      <c r="J18" s="17">
+        <f>365.25*H9</f>
+        <v>-3.4337857375058132</v>
+      </c>
+      <c r="K18" s="17">
+        <f>J18-0.01</f>
+        <v>-3.443785737505813</v>
+      </c>
+      <c r="L18" s="17">
+        <f>AVERAGE(K18:K26)</f>
+        <v>0.70023905567271005</v>
+      </c>
       <c r="M18" s="5"/>
+      <c r="N18">
+        <f>AVERAGE(H9:H16)</f>
+        <v>2.1841723138447604E-3</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C19" s="5"/>
       <c r="F19" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="20">
+      <c r="G19" s="48">
         <f>J16</f>
         <v>1.0176269310457635</v>
       </c>
-      <c r="H19" s="20">
+      <c r="H19" s="48">
         <f>L16</f>
         <v>1.0176269310457635</v>
+      </c>
+      <c r="J19" s="17">
+        <f t="shared" ref="J19:J26" si="8">365.25*H10</f>
+        <v>0.24689898182666467</v>
+      </c>
+      <c r="K19" s="17">
+        <f t="shared" ref="K19:K25" si="9">J19-0.01</f>
+        <v>0.23689898182666466</v>
+      </c>
+      <c r="L19">
+        <f>_xlfn.STDEV.S(K18:K26)</f>
+        <v>2.4325320751047155</v>
+      </c>
+      <c r="N19">
+        <f>_xlfn.STDEV.S(H9:H16)</f>
+        <v>7.0781383450986704E-3</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
@@ -6665,53 +6719,111 @@
       <c r="F20" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="49">
         <f>G19^(1/COUNT(G9:G16))-1</f>
         <v>2.186559355780382E-3</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="49">
         <f>H19^(1/COUNT(L9:L16))-1</f>
         <v>2.186559355780382E-3</v>
       </c>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
+      <c r="J20" s="17">
+        <f t="shared" si="8"/>
+        <v>0.25890811922203683</v>
+      </c>
+      <c r="K20" s="17">
+        <f t="shared" si="9"/>
+        <v>0.24890811922203682</v>
+      </c>
       <c r="L20" s="44"/>
-      <c r="N20" s="43"/>
+      <c r="N20" s="43">
+        <f>N18/N19</f>
+        <v>0.30858005415466522</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D21" s="5"/>
+      <c r="J21" s="17">
+        <f t="shared" si="8"/>
+        <v>4.6780681872169598</v>
+      </c>
+      <c r="K21" s="17">
+        <f t="shared" si="9"/>
+        <v>4.66806818721696</v>
+      </c>
+      <c r="L21">
+        <f>L18/L19</f>
+        <v>0.28786426408891902</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="F22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G22" s="4">
-        <f>AVERAGE(G9:G16)/_xlfn.STDEV.S(G9:G16)</f>
-        <v>0.3112579807659363</v>
+        <f>(AVERAGE(G9:G16)-0.01)/_xlfn.STDEV.S(G9:G16)</f>
+        <v>-1.0980867636013225</v>
+      </c>
+      <c r="J22" s="17">
+        <f t="shared" si="8"/>
+        <v>1.1028474125939736</v>
+      </c>
+      <c r="K22" s="17">
+        <f t="shared" si="9"/>
+        <v>1.0928474125939736</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C23" s="22"/>
       <c r="F23" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="G23" s="4">
-        <f>(AVERAGE(G9:G16)-0.01)/_xlfn.STDEV.S(G9:G16)</f>
-        <v>-1.0980867636013225</v>
+        <f>(AVERAGE(H9:H16)-0.01)/_xlfn.STDEV.S(H9:H16)*SQRT(365.2422)</f>
+        <v>-21.103107156945686</v>
+      </c>
+      <c r="J23" s="17">
+        <f t="shared" si="8"/>
+        <v>-0.96979844886422917</v>
+      </c>
+      <c r="K23" s="17">
+        <f t="shared" si="9"/>
+        <v>-0.97979844886422918</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G24" s="4"/>
+      <c r="J24" s="17">
+        <f t="shared" si="8"/>
+        <v>3.9520068114662004</v>
+      </c>
+      <c r="K24" s="17">
+        <f t="shared" si="9"/>
+        <v>3.9420068114662006</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F25" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G25" s="4">
-        <f>(E8-E6)/E6</f>
-        <v>2.4735087217370054E-3</v>
+        <f>(E10-E9)/E9</f>
+        <v>6.7620109268352803E-4</v>
+      </c>
+      <c r="J25" s="17">
+        <f t="shared" si="8"/>
+        <v>0.54700617509859673</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J26" s="17"/>
+      <c r="K26" s="17">
+        <f>J25-0.01</f>
+        <v>0.53700617509859672</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
@@ -6770,7 +6882,7 @@
         <v>1100000</v>
       </c>
       <c r="D31">
-        <f>G6</f>
+        <f t="shared" ref="D31:D41" si="10">G6</f>
         <v>0</v>
       </c>
       <c r="E31" s="23">
@@ -6791,7 +6903,7 @@
         <v>2100000</v>
       </c>
       <c r="D32">
-        <f>G7</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="E32" s="23">
@@ -6816,7 +6928,7 @@
         <v>11689</v>
       </c>
       <c r="B33" s="23">
-        <f t="shared" ref="B33:B41" si="8">1000000</f>
+        <f t="shared" ref="B33:B41" si="11">1000000</f>
         <v>1000000</v>
       </c>
       <c r="C33">
@@ -6824,19 +6936,19 @@
         <v>3100000</v>
       </c>
       <c r="D33">
-        <f>G8</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="E33" s="23">
-        <f t="shared" ref="E33:E41" si="9">E32*(1+D33)+B33</f>
+        <f t="shared" ref="E33:E41" si="12">E32*(1+D33)+B33</f>
         <v>3100000</v>
       </c>
       <c r="F33" s="21">
-        <f t="shared" ref="F33:F41" si="10">E33/E32-1</f>
+        <f t="shared" ref="F33:F41" si="13">E33/E32-1</f>
         <v>0.47619047619047628</v>
       </c>
       <c r="G33" s="25">
-        <f t="shared" ref="G33:G41" si="11">F33+1</f>
+        <f t="shared" ref="G33:G41" si="14">F33+1</f>
         <v>1.4761904761904763</v>
       </c>
       <c r="H33" s="17">
@@ -6849,7 +6961,7 @@
         <v>12055</v>
       </c>
       <c r="B34" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1000000</v>
       </c>
       <c r="C34">
@@ -6857,19 +6969,19 @@
         <v>4100000</v>
       </c>
       <c r="D34">
-        <f>G9</f>
+        <f t="shared" si="10"/>
         <v>-9.357139928022673E-3</v>
       </c>
       <c r="E34" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>4070992.8662231299</v>
       </c>
       <c r="F34" s="21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.3132235052332677</v>
       </c>
       <c r="G34" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1.3132235052332677</v>
       </c>
       <c r="H34" s="17">
@@ -6882,7 +6994,7 @@
         <v>12420</v>
       </c>
       <c r="B35" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1000000</v>
       </c>
       <c r="C35">
@@ -6890,19 +7002,19 @@
         <v>5100000</v>
       </c>
       <c r="D35">
-        <f>G10</f>
+        <f t="shared" si="10"/>
         <v>6.7620109268351491E-4</v>
       </c>
       <c r="E35" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>5073745.6760475766</v>
       </c>
       <c r="F35" s="21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.24631652345653765</v>
       </c>
       <c r="G35" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1.2463165234565377</v>
       </c>
       <c r="H35" s="17">
@@ -6915,7 +7027,7 @@
         <v>12785</v>
       </c>
       <c r="B36" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1000000</v>
       </c>
       <c r="C36">
@@ -6923,19 +7035,19 @@
         <v>6100000</v>
       </c>
       <c r="D36">
-        <f>G11</f>
+        <f t="shared" si="10"/>
         <v>7.0910309281613237E-4</v>
       </c>
       <c r="E36" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>6077343.4847986242</v>
       </c>
       <c r="F36" s="21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.19780215107920918</v>
       </c>
       <c r="G36" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1.1978021510792092</v>
       </c>
       <c r="H36" s="17">
@@ -6948,7 +7060,7 @@
         <v>13150</v>
       </c>
       <c r="B37" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1000000</v>
       </c>
       <c r="C37">
@@ -6956,19 +7068,19 @@
         <v>7100000</v>
       </c>
       <c r="D37">
-        <f>G12</f>
+        <f t="shared" si="10"/>
         <v>1.2890224506745485E-2</v>
       </c>
       <c r="E37" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>7155681.8067222852</v>
       </c>
       <c r="F37" s="21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.17743580309734508</v>
       </c>
       <c r="G37" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1.1774358030973451</v>
       </c>
       <c r="H37" s="17">
@@ -6981,7 +7093,7 @@
         <v>13516</v>
       </c>
       <c r="B38" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1000000</v>
       </c>
       <c r="C38">
@@ -6989,19 +7101,19 @@
         <v>8100000</v>
       </c>
       <c r="D38">
-        <f>G13</f>
+        <f t="shared" si="10"/>
         <v>3.0239947318970728E-3</v>
       </c>
       <c r="E38" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>8177320.5508089447</v>
       </c>
       <c r="F38" s="21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.14277308182246151</v>
       </c>
       <c r="G38" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1.1427730818224615</v>
       </c>
       <c r="H38" s="17">
@@ -7014,7 +7126,7 @@
         <v>13881</v>
       </c>
       <c r="B39" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1000000</v>
       </c>
       <c r="C39">
@@ -7022,19 +7134,19 @@
         <v>9100000</v>
       </c>
       <c r="D39">
-        <f>G14</f>
+        <f t="shared" si="10"/>
         <v>-2.6516416178182789E-3</v>
       </c>
       <c r="E39" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>9155637.2273141779</v>
       </c>
       <c r="F39" s="21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.11963780439161731</v>
       </c>
       <c r="G39" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1.1196378043916173</v>
       </c>
       <c r="H39" s="17">
@@ -7047,7 +7159,7 @@
         <v>14246</v>
       </c>
       <c r="B40" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1000000</v>
       </c>
       <c r="C40">
@@ -7055,19 +7167,19 @@
         <v>10100000</v>
       </c>
       <c r="D40">
-        <f>G15</f>
+        <f t="shared" si="10"/>
         <v>1.0878752906358091E-2</v>
       </c>
       <c r="E40" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>10255239.142410383</v>
       </c>
       <c r="F40" s="21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.12010107956393723</v>
       </c>
       <c r="G40" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1.1201010795639372</v>
       </c>
       <c r="H40" s="17">
@@ -7080,7 +7192,7 @@
         <v>14611</v>
       </c>
       <c r="B41" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1000000</v>
       </c>
       <c r="C41">
@@ -7088,19 +7200,19 @@
         <v>11100000</v>
       </c>
       <c r="D41">
-        <f>G16</f>
+        <f t="shared" si="10"/>
         <v>1.4987432818573954E-3</v>
       </c>
       <c r="E41" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>11270609.113178911</v>
       </c>
       <c r="F41" s="21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>9.9009877455658923E-2</v>
       </c>
       <c r="G41" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1.0990098774556589</v>
       </c>
       <c r="H41" s="17">
@@ -7490,11 +7602,11 @@
         <v>-0.14228399999999999</v>
       </c>
       <c r="O10" s="32">
-        <f t="shared" ref="O10:O18" si="6">M10+1</f>
+        <f t="shared" ref="O10:O17" si="6">M10+1</f>
         <v>0.86737472516283098</v>
       </c>
       <c r="P10" s="32">
-        <f t="shared" ref="P10:P18" si="7">N10</f>
+        <f t="shared" ref="P10:P17" si="7">N10</f>
         <v>-0.14228399999999999</v>
       </c>
       <c r="Q10">
@@ -8121,7 +8233,7 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="F27" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G27" s="4">
         <f>(E10-E8)/E8</f>
@@ -9240,7 +9352,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G15" s="19">
         <v>14246</v>
@@ -9278,7 +9390,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G16" s="19">
         <v>14611</v>
@@ -9316,7 +9428,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="N17"/>
     </row>
@@ -9325,7 +9437,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J18" s="7"/>
     </row>
@@ -9334,7 +9446,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J19" s="7"/>
     </row>
@@ -9343,7 +9455,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C20" s="26"/>
       <c r="J20" s="7"/>
@@ -9364,7 +9476,7 @@
         <v>17</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C22" s="26"/>
       <c r="D22" s="16"/>
@@ -9410,7 +9522,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C23" s="26"/>
       <c r="H23" s="10">
@@ -10914,10 +11026,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1061419-436F-4506-9C6C-1EBD96D9F722}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="B1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="B1" sqref="B1:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10926,211 +11038,92 @@
     <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1">
-        <v>0.18662799999999999</v>
-      </c>
-      <c r="D1" s="38">
-        <v>10593</v>
-      </c>
-      <c r="E1">
-        <v>0</v>
-      </c>
-      <c r="G1" s="38">
-        <v>10593</v>
-      </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2">
-        <v>1.4356000000000001E-2</v>
-      </c>
-      <c r="D2" s="38">
-        <v>10958</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="38">
-        <v>10958</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B1" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="B3">
-        <v>1.4460000000000001E-2</v>
-      </c>
-      <c r="D3" s="38">
-        <v>11323</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="38">
-        <v>11323</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="D1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="I1" s="20"/>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="B4">
-        <v>1.445953</v>
-      </c>
-      <c r="D4" s="38">
-        <v>11688</v>
-      </c>
-      <c r="E4">
-        <v>-0.47318900000000003</v>
-      </c>
-      <c r="G4" s="38">
-        <v>11688</v>
-      </c>
-      <c r="H4">
-        <v>-0.37698799999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D5" s="38">
-        <v>12054</v>
-      </c>
-      <c r="E5">
-        <v>-0.136354</v>
-      </c>
-      <c r="G5" s="38">
-        <v>12054</v>
-      </c>
-      <c r="H5">
-        <v>-0.127466</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D6" s="38">
-        <v>12419</v>
-      </c>
-      <c r="E6">
-        <v>0.40719499999999997</v>
-      </c>
-      <c r="G6" s="38">
-        <v>12419</v>
-      </c>
-      <c r="H6">
-        <v>0.50259699999999996</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D7" s="38">
-        <v>12784</v>
-      </c>
-      <c r="E7">
-        <v>-2.562E-2</v>
-      </c>
-      <c r="G7" s="38">
-        <v>12784</v>
-      </c>
-      <c r="H7">
-        <v>-2.5295000000000002E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D8" s="38">
-        <v>13149</v>
-      </c>
-      <c r="E8">
-        <v>0.36797000000000002</v>
-      </c>
-      <c r="G8" s="38">
-        <v>13149</v>
-      </c>
-      <c r="H8">
-        <v>0.44479800000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D9" s="38">
-        <v>13515</v>
-      </c>
-      <c r="E9">
-        <v>0.304342</v>
-      </c>
-      <c r="G9" s="38">
-        <v>13515</v>
-      </c>
-      <c r="H9">
-        <v>0.35573300000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D10" s="38">
-        <v>13880</v>
-      </c>
-      <c r="E10">
-        <v>-0.359983</v>
-      </c>
-      <c r="G10" s="38">
-        <v>13880</v>
-      </c>
-      <c r="H10">
-        <v>-0.30231200000000003</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D11" s="38">
-        <v>14245</v>
-      </c>
-      <c r="E11">
-        <v>0.17676800000000001</v>
-      </c>
-      <c r="G11" s="38">
-        <v>14245</v>
-      </c>
-      <c r="H11">
-        <v>0.193354</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D12" s="38">
-        <v>14610</v>
-      </c>
-      <c r="E12">
-        <v>2.2928E-2</v>
-      </c>
-      <c r="G12" s="38">
-        <v>14610</v>
-      </c>
-      <c r="H12">
-        <v>2.3192999999999998E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D13" s="38">
-        <v>14976</v>
-      </c>
-      <c r="E13">
-        <v>-9.7429000000000002E-2</v>
-      </c>
-      <c r="G13" s="38">
-        <v>14976</v>
-      </c>
-      <c r="H13">
-        <v>-9.2832999999999999E-2</v>
-      </c>
+      <c r="D2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="I2" s="20"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="I3" s="20"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="I4" s="20"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="I5" s="20"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="I6" s="20"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="I7" s="20"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="I8" s="20"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="38"/>
+      <c r="G9" s="38"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D10" s="38"/>
+      <c r="G10" s="38"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D11" s="38"/>
+      <c r="G11" s="38"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D12" s="38"/>
+      <c r="G12" s="38"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D13" s="38"/>
+      <c r="G13" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Report and results check
</commit_message>
<xml_diff>
--- a/misc analysis/Results analysis (Annual Data).xlsx
+++ b/misc analysis/Results analysis (Annual Data).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feder\Desktop\portfolio-allocation\misc analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fega\Desktop\portfolio-allocation\misc analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED4F3B9-2871-48E7-8A02-E5F3AD316D91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C84DA2F-15F4-4351-AB20-E0C16E4A22E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{161C5C75-020D-46B4-9A37-BBAEE0A65B1A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{161C5C75-020D-46B4-9A37-BBAEE0A65B1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily from backtrader" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="62">
   <si>
     <t>DATE</t>
   </si>
@@ -207,7 +207,22 @@
     <t xml:space="preserve">             (datetime.datetime(2019, 2, 19, 0, 0), 0.0014972815135696387)])</t>
   </si>
   <si>
-    <t>SR (r=1%) logret</t>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>skew</t>
+  </si>
+  <si>
+    <t>kurt</t>
+  </si>
+  <si>
+    <t>annualized</t>
+  </si>
+  <si>
+    <t>Logret (annualized)</t>
   </si>
 </sst>
 </file>
@@ -220,7 +235,7 @@
     <numFmt numFmtId="165" formatCode="0.000000"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="0.00000000000000"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="0.0%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -259,7 +274,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,6 +314,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -346,7 +367,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -395,8 +416,15 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="3" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="3" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -483,10 +511,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Daily calculated'!$E$8:$E$16</c:f>
+              <c:f>'Daily calculated'!$E$8:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>2731.610107</c:v>
                 </c:pt>
@@ -512,6 +540,9 @@
                   <c:v>2775.6000979999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>2775.6000979999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>2779.76001</c:v>
                 </c:pt>
               </c:numCache>
@@ -3780,13 +3811,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>176213</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>23813</xdr:rowOff>
@@ -3818,16 +3849,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>166688</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>119062</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>83344</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>14288</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>497681</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>121444</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3856,16 +3887,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>402432</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3880,8 +3911,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1644015" y="161925"/>
-          <a:ext cx="1160145" cy="3619500"/>
+          <a:off x="18642807" y="590550"/>
+          <a:ext cx="1895474" cy="3390900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5960,10 +5991,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ADAAC33-8865-4FC7-A80E-FBB32674269F}">
-  <dimension ref="A3:R48"/>
+  <dimension ref="A3:S48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5974,10 +6005,12 @@
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -5985,13 +6018,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E4" s="5"/>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -6016,20 +6049,23 @@
       <c r="H5" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17" t="s">
+      <c r="I5" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="17"/>
       <c r="L5" s="17"/>
-      <c r="M5" t="s">
+      <c r="M5" s="17"/>
+      <c r="N5" t="s">
         <v>11</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="38">
         <v>43500</v>
       </c>
@@ -6050,25 +6086,26 @@
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
-      <c r="I6" s="17"/>
+      <c r="I6" s="20"/>
       <c r="J6" s="17"/>
       <c r="K6" s="17"/>
       <c r="L6" s="17"/>
-      <c r="M6" s="46"/>
-      <c r="O6" s="32">
-        <f t="shared" ref="O6" si="0">M6+1</f>
+      <c r="M6" s="17"/>
+      <c r="N6" s="46"/>
+      <c r="P6" s="32">
+        <f t="shared" ref="P6" si="0">N6+1</f>
         <v>1</v>
       </c>
-      <c r="P6" s="32">
-        <f t="shared" ref="P6" si="1">N6</f>
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <f>PRODUCT($O$6:O6)</f>
+      <c r="Q6" s="32">
+        <f t="shared" ref="Q6" si="1">O6</f>
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <f>PRODUCT($P$6:P6)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="38">
         <v>43501</v>
       </c>
@@ -6089,29 +6126,30 @@
       </c>
       <c r="G7" s="33"/>
       <c r="H7" s="20"/>
-      <c r="I7" s="17"/>
+      <c r="I7" s="20"/>
       <c r="J7" s="17"/>
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
-      <c r="M7" s="46"/>
-      <c r="O7" s="32">
-        <f>M7+1</f>
+      <c r="M7" s="17"/>
+      <c r="N7" s="46"/>
+      <c r="P7" s="32">
+        <f>N7+1</f>
         <v>1</v>
       </c>
-      <c r="P7" s="32">
-        <f>N7</f>
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <f>PRODUCT($O$6:O7)</f>
+      <c r="Q7" s="32">
+        <f>O7</f>
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <f>PRODUCT($P$6:P7)</f>
         <v>1</v>
       </c>
-      <c r="R7">
-        <f>EXP(SUM($P$7:P7))</f>
+      <c r="S7">
+        <f>EXP(SUM($Q$7:Q7))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="38">
         <v>43502</v>
       </c>
@@ -6132,29 +6170,30 @@
       </c>
       <c r="G8" s="33"/>
       <c r="H8" s="20"/>
-      <c r="I8" s="17"/>
+      <c r="I8" s="20"/>
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
       <c r="L8" s="17"/>
-      <c r="M8" s="46"/>
-      <c r="O8" s="32">
-        <f t="shared" ref="O8:O15" si="2">M8+1</f>
+      <c r="M8" s="17"/>
+      <c r="N8" s="46"/>
+      <c r="P8" s="32">
+        <f t="shared" ref="P8:P15" si="2">N8+1</f>
         <v>1</v>
       </c>
-      <c r="P8" s="32">
-        <f t="shared" ref="P8:P15" si="3">N8</f>
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <f>PRODUCT($O$6:O8)</f>
+      <c r="Q8" s="32">
+        <f t="shared" ref="Q8:Q15" si="3">O8</f>
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <f>PRODUCT($P$6:P8)</f>
         <v>1</v>
       </c>
-      <c r="R8">
-        <f>EXP(SUM($P$7:P8))</f>
+      <c r="S8">
+        <f>EXP(SUM($Q$7:Q8))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="38">
         <v>43503</v>
       </c>
@@ -6181,43 +6220,50 @@
         <f t="shared" ref="H9:H16" si="5">LN(E9/E8)</f>
         <v>-9.4011929842732732E-3</v>
       </c>
-      <c r="I9" s="17">
-        <f t="shared" ref="I9:I16" si="6">G9+1</f>
+      <c r="I9" s="20">
+        <f>H9*260</f>
+        <v>-2.4443101759110508</v>
+      </c>
+      <c r="J9" s="17">
+        <f t="shared" ref="J9:J16" si="6">G9+1</f>
         <v>0.99064286007197733</v>
       </c>
-      <c r="J9" s="17">
-        <f>PRODUCT($I$7:I9)</f>
+      <c r="K9" s="17">
+        <f>PRODUCT($J$7:J9)</f>
         <v>0.99064286007197733</v>
       </c>
-      <c r="K9" s="17">
+      <c r="L9" s="17">
         <f>SUM($H$7:H9)</f>
         <v>-9.4011929842732732E-3</v>
       </c>
-      <c r="L9" s="17">
-        <f t="shared" ref="L9:L16" si="7">EXP(K9)</f>
+      <c r="M9" s="17">
+        <f t="shared" ref="M9:M16" si="7">EXP(L9)</f>
         <v>0.99064286007197733</v>
       </c>
-      <c r="M9" s="46">
+      <c r="N9" s="6">
         <v>-9.3550000000000005E-3</v>
       </c>
-      <c r="O9" s="32">
-        <f t="shared" si="2"/>
-        <v>0.990645</v>
-      </c>
-      <c r="P9" s="32">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <f>PRODUCT($O$6:O9)</f>
-        <v>0.990645</v>
-      </c>
-      <c r="R9">
-        <f>EXP(SUM($P$7:P9))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O9" s="6">
+        <v>-9.3989999999999994E-3</v>
+      </c>
+      <c r="P9" s="32" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q9" s="32" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R9" t="e">
+        <f>PRODUCT($P$6:P9)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S9" t="e">
+        <f>EXP(SUM($Q$7:Q9))</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="38">
         <v>43504</v>
       </c>
@@ -6244,43 +6290,50 @@
         <f t="shared" si="5"/>
         <v>6.7597257173624824E-4</v>
       </c>
-      <c r="I10" s="17">
+      <c r="I10" s="20">
+        <f t="shared" ref="I10:I17" si="8">H10*260</f>
+        <v>0.17575286865142453</v>
+      </c>
+      <c r="J10" s="17">
         <f t="shared" si="6"/>
         <v>1.0006762010926835</v>
       </c>
-      <c r="J10" s="17">
-        <f>PRODUCT($I$7:I10)</f>
+      <c r="K10" s="17">
+        <f>PRODUCT($J$7:J10)</f>
         <v>0.99131273385641716</v>
       </c>
-      <c r="K10" s="17">
+      <c r="L10" s="17">
         <f>SUM($H$7:H10)</f>
         <v>-8.7252204125370242E-3</v>
       </c>
-      <c r="L10" s="17">
+      <c r="M10" s="17">
         <f t="shared" si="7"/>
         <v>0.99131273385641716</v>
       </c>
-      <c r="M10" s="46">
+      <c r="N10" s="6">
         <v>6.7599999999999995E-4</v>
       </c>
-      <c r="O10" s="32">
-        <f t="shared" si="2"/>
-        <v>1.0006759999999999</v>
-      </c>
-      <c r="P10" s="32">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <f>PRODUCT($O$6:O10)</f>
-        <v>0.9913146760199999</v>
-      </c>
-      <c r="R10">
-        <f>EXP(SUM($P$7:P10))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O10" s="6">
+        <v>6.7599999999999995E-4</v>
+      </c>
+      <c r="P10" s="32" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q10" s="32" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R10" t="e">
+        <f>PRODUCT($P$6:P10)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S10" t="e">
+        <f>EXP(SUM($Q$7:Q10))</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="38">
         <v>43507</v>
       </c>
@@ -6307,43 +6360,50 @@
         <f t="shared" si="5"/>
         <v>7.0885179800694539E-4</v>
       </c>
-      <c r="I11" s="17">
+      <c r="I11" s="20">
+        <f t="shared" si="8"/>
+        <v>0.18430146748180581</v>
+      </c>
+      <c r="J11" s="17">
         <f t="shared" si="6"/>
         <v>1.0007091030928161</v>
       </c>
-      <c r="J11" s="17">
-        <f>PRODUCT($I$7:I11)</f>
+      <c r="K11" s="17">
+        <f>PRODUCT($J$7:J11)</f>
         <v>0.9920156767819428</v>
       </c>
-      <c r="K11" s="17">
+      <c r="L11" s="17">
         <f>SUM($H$7:H11)</f>
         <v>-8.016368614530079E-3</v>
       </c>
-      <c r="L11" s="17">
+      <c r="M11" s="17">
         <f t="shared" si="7"/>
         <v>0.99201567678194269</v>
       </c>
-      <c r="M11" s="46">
+      <c r="N11" s="6">
         <v>7.0899999999999999E-4</v>
       </c>
-      <c r="O11" s="32">
-        <f t="shared" si="2"/>
-        <v>1.0007090000000001</v>
-      </c>
-      <c r="P11" s="32">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <f>PRODUCT($O$6:O11)</f>
-        <v>0.99201751812529815</v>
-      </c>
-      <c r="R11">
-        <f>EXP(SUM($P$7:P11))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O11" s="6">
+        <v>7.0899999999999999E-4</v>
+      </c>
+      <c r="P11" s="32" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q11" s="32" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R11" t="e">
+        <f>PRODUCT($P$6:P11)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S11" t="e">
+        <f>EXP(SUM($Q$7:Q11))</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="38">
         <v>43508</v>
       </c>
@@ -6370,43 +6430,50 @@
         <f t="shared" si="5"/>
         <v>1.2807852668629596E-2</v>
       </c>
-      <c r="I12" s="17">
+      <c r="I12" s="20">
+        <f t="shared" si="8"/>
+        <v>3.330041693843695</v>
+      </c>
+      <c r="J12" s="17">
         <f t="shared" si="6"/>
         <v>1.0128902245067455</v>
       </c>
-      <c r="J12" s="17">
-        <f>PRODUCT($I$7:I12)</f>
+      <c r="K12" s="17">
+        <f>PRODUCT($J$7:J12)</f>
         <v>1.0048029815698731</v>
       </c>
-      <c r="K12" s="17">
+      <c r="L12" s="17">
         <f>SUM($H$7:H12)</f>
         <v>4.7914840540995169E-3</v>
       </c>
-      <c r="L12" s="17">
+      <c r="M12" s="17">
         <f t="shared" si="7"/>
         <v>1.0048029815698731</v>
       </c>
-      <c r="M12" s="46">
+      <c r="N12" s="6">
         <v>1.2886999999999999E-2</v>
       </c>
-      <c r="O12" s="32">
-        <f t="shared" si="2"/>
-        <v>1.0128870000000001</v>
-      </c>
-      <c r="P12" s="32">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <f>PRODUCT($O$6:O12)</f>
-        <v>1.004801647881379</v>
-      </c>
-      <c r="R12">
-        <f>EXP(SUM($P$7:P12))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O12" s="51">
+        <v>1.2805E-2</v>
+      </c>
+      <c r="P12" s="32" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q12" s="32" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R12" t="e">
+        <f>PRODUCT($P$6:P12)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S12" t="e">
+        <f>EXP(SUM($Q$7:Q12))</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="38">
         <v>43509</v>
       </c>
@@ -6433,43 +6500,50 @@
         <f t="shared" si="5"/>
         <v>3.0194316566570117E-3</v>
       </c>
-      <c r="I13" s="17">
+      <c r="I13" s="20">
+        <f t="shared" si="8"/>
+        <v>0.78505223073082309</v>
+      </c>
+      <c r="J13" s="17">
         <f t="shared" si="6"/>
         <v>1.0030239947318971</v>
       </c>
-      <c r="J13" s="17">
-        <f>PRODUCT($I$7:I13)</f>
+      <c r="K13" s="17">
+        <f>PRODUCT($J$7:J13)</f>
         <v>1.0078415004927348</v>
       </c>
-      <c r="K13" s="17">
+      <c r="L13" s="17">
         <f>SUM($H$7:H13)</f>
         <v>7.8109157107565282E-3</v>
       </c>
-      <c r="L13" s="17">
+      <c r="M13" s="17">
         <f t="shared" si="7"/>
         <v>1.0078415004927348</v>
       </c>
-      <c r="M13" s="46">
+      <c r="N13" s="6">
         <v>3.0230000000000001E-3</v>
       </c>
-      <c r="O13" s="32">
-        <f t="shared" si="2"/>
-        <v>1.003023</v>
-      </c>
-      <c r="P13" s="32">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <f>PRODUCT($O$6:O13)</f>
-        <v>1.0078391632629244</v>
-      </c>
-      <c r="R13">
-        <f>EXP(SUM($P$7:P13))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O13" s="6">
+        <v>3.019E-3</v>
+      </c>
+      <c r="P13" s="32" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q13" s="32" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R13" t="e">
+        <f>PRODUCT($P$6:P13)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S13" t="e">
+        <f>EXP(SUM($Q$7:Q13))</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="38">
         <v>43510</v>
       </c>
@@ -6496,43 +6570,50 @@
         <f t="shared" si="5"/>
         <v>-2.6551634465824207E-3</v>
       </c>
-      <c r="I14" s="17">
+      <c r="I14" s="20">
+        <f t="shared" si="8"/>
+        <v>-0.69034249611142939</v>
+      </c>
+      <c r="J14" s="17">
         <f t="shared" si="6"/>
         <v>0.99734835838218172</v>
       </c>
-      <c r="J14" s="17">
-        <f>PRODUCT($I$7:I14)</f>
+      <c r="K14" s="17">
+        <f>PRODUCT($J$7:J14)</f>
         <v>1.0051690660258639</v>
       </c>
-      <c r="K14" s="17">
+      <c r="L14" s="17">
         <f>SUM($H$7:H14)</f>
         <v>5.1557522641741075E-3</v>
       </c>
-      <c r="L14" s="17">
+      <c r="M14" s="17">
         <f t="shared" si="7"/>
         <v>1.0051690660258639</v>
       </c>
-      <c r="M14" s="46">
+      <c r="N14" s="6">
         <v>-2.6510000000000001E-3</v>
       </c>
-      <c r="O14" s="32">
-        <f t="shared" si="2"/>
-        <v>0.99734900000000004</v>
-      </c>
-      <c r="P14" s="32">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <f>PRODUCT($O$6:O14)</f>
-        <v>1.0051673816411144</v>
-      </c>
-      <c r="R14">
-        <f>EXP(SUM($P$7:P14))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O14" s="6">
+        <v>-2.6549999999999998E-3</v>
+      </c>
+      <c r="P14" s="32" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q14" s="32" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R14" t="e">
+        <f>PRODUCT($P$6:P14)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S14" t="e">
+        <f>EXP(SUM($Q$7:Q14))</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="38">
         <v>43511</v>
       </c>
@@ -6559,274 +6640,390 @@
         <f t="shared" si="5"/>
         <v>1.0820004959524163E-2</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I15" s="20">
+        <f t="shared" si="8"/>
+        <v>2.8132012894762823</v>
+      </c>
+      <c r="J15" s="17">
         <f t="shared" si="6"/>
         <v>1.0108787529063581</v>
       </c>
-      <c r="J15" s="17">
-        <f>PRODUCT($I$7:I15)</f>
+      <c r="K15" s="17">
+        <f>PRODUCT($J$7:J15)</f>
         <v>1.0161040519242739</v>
       </c>
-      <c r="K15" s="17">
+      <c r="L15" s="17">
         <f>SUM($H$7:H15)</f>
         <v>1.5975757223698268E-2</v>
       </c>
-      <c r="L15" s="17">
+      <c r="M15" s="17">
         <f t="shared" si="7"/>
         <v>1.0161040519242739</v>
       </c>
-      <c r="M15" s="46">
+      <c r="N15" s="6">
         <v>1.0876E-2</v>
       </c>
-      <c r="O15" s="32">
-        <f t="shared" si="2"/>
-        <v>1.0108760000000001</v>
-      </c>
-      <c r="P15" s="32">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <f>PRODUCT($O$6:O15)</f>
-        <v>1.0160995820838432</v>
-      </c>
-      <c r="R15">
-        <f>EXP(SUM($P$7:P15))</f>
+      <c r="O15" s="6">
+        <v>1.0817999999999999E-2</v>
+      </c>
+      <c r="P15" s="32" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q15" s="32" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R15" t="e">
+        <f>PRODUCT($P$6:P15)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S15" t="e">
+        <f>EXP(SUM($Q$7:Q15))</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="52">
+        <v>43515</v>
+      </c>
+      <c r="B16" s="53">
+        <f>B15</f>
+        <v>2775.6000979999999</v>
+      </c>
+      <c r="C16" s="53">
+        <f t="shared" ref="C16:F16" si="9">C15</f>
+        <v>2775.6000979999999</v>
+      </c>
+      <c r="D16" s="53">
+        <f t="shared" si="9"/>
+        <v>2775.6000979999999</v>
+      </c>
+      <c r="E16" s="53">
+        <f t="shared" si="9"/>
+        <v>2775.6000979999999</v>
+      </c>
+      <c r="F16" s="53">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="54">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="55">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="55">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="53">
+        <f t="shared" ref="J16" si="10">G16+1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="38">
+      <c r="K16" s="53">
+        <f>PRODUCT($J$7:J16)</f>
+        <v>1.0161040519242739</v>
+      </c>
+      <c r="L16" s="53">
+        <f>SUM($H$7:H16)</f>
+        <v>1.5975757223698268E-2</v>
+      </c>
+      <c r="M16" s="53">
+        <f t="shared" ref="M16" si="11">EXP(L16)</f>
+        <v>1.0161040519242739</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16" s="6">
+        <v>0</v>
+      </c>
+      <c r="P16" s="32" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q16" s="32" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R16" t="e">
+        <f>PRODUCT($P$6:P16)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S16" t="e">
+        <f>EXP(SUM($Q$7:Q16))</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="38">
         <v>43515</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>2779.76001</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>2779.76001</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>2779.76001</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>2779.76001</v>
       </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16" s="33">
-        <f t="shared" si="4"/>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" s="33">
+        <f>E17/E15-1</f>
         <v>1.4987432818573954E-3</v>
       </c>
-      <c r="H16" s="20">
-        <f t="shared" si="5"/>
+      <c r="H17" s="20">
+        <f>LN(E17/E15)</f>
         <v>1.4976212870598132E-3</v>
       </c>
-      <c r="I16" s="17">
-        <f t="shared" si="6"/>
+      <c r="I17" s="20">
+        <f t="shared" si="8"/>
+        <v>0.38938153463555142</v>
+      </c>
+      <c r="J17" s="17">
+        <f>G17+1</f>
         <v>1.0014987432818574</v>
       </c>
-      <c r="J16" s="17">
-        <f>PRODUCT($I$7:I16)</f>
+      <c r="K17" s="17">
+        <f>PRODUCT($J$7:J17)</f>
         <v>1.0176269310457635</v>
       </c>
-      <c r="K16" s="17">
-        <f>SUM($H$7:H16)</f>
+      <c r="L17" s="17">
+        <f>SUM($H$7:H17)</f>
         <v>1.7473378510758083E-2</v>
       </c>
-      <c r="L16" s="17">
-        <f t="shared" si="7"/>
+      <c r="M17" s="17">
+        <f>EXP(L17)</f>
         <v>1.0176269310457635</v>
       </c>
-      <c r="M16" s="46">
+      <c r="N17">
         <v>1.498E-3</v>
       </c>
-      <c r="O16" s="32">
-        <f>M16+1</f>
-        <v>1.001498</v>
-      </c>
-      <c r="P16" s="32">
-        <f>N16</f>
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <f>PRODUCT($O$6:O16)</f>
-        <v>1.0176216992578049</v>
-      </c>
-      <c r="R16">
-        <f>EXP(SUM($P$7:P16))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G18" t="s">
-        <v>37</v>
-      </c>
-      <c r="H18" t="s">
-        <v>38</v>
-      </c>
-      <c r="J18" s="17">
-        <f>365.25*H9</f>
-        <v>-3.4337857375058132</v>
-      </c>
-      <c r="K18" s="17">
-        <f>J18-0.01</f>
-        <v>-3.443785737505813</v>
-      </c>
-      <c r="L18" s="17">
-        <f>AVERAGE(K18:K26)</f>
-        <v>0.70023905567271005</v>
-      </c>
-      <c r="M18" s="5"/>
-      <c r="N18">
-        <f>AVERAGE(H9:H16)</f>
-        <v>2.1841723138447604E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <v>1.4970000000000001E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F18" s="6"/>
+      <c r="G18" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" s="7">
+        <f>AVERAGE(H9:H17)</f>
+        <v>1.9414865011953425E-3</v>
+      </c>
+      <c r="I18" s="7">
+        <f>AVERAGE(I9:I17)</f>
+        <v>0.50478649031078904</v>
+      </c>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="O18" s="7">
+        <f>AVERAGE(O9:O17)</f>
+        <v>1.9411111111111111E-3</v>
+      </c>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C19" s="5"/>
-      <c r="F19" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19" s="48">
-        <f>J16</f>
-        <v>1.0176269310457635</v>
-      </c>
-      <c r="H19" s="48">
-        <f>L16</f>
-        <v>1.0176269310457635</v>
-      </c>
-      <c r="J19" s="17">
-        <f t="shared" ref="J19:J25" si="8">365.25*H10</f>
-        <v>0.24689898182666467</v>
-      </c>
-      <c r="K19" s="17">
-        <f t="shared" ref="K19:K24" si="9">J19-0.01</f>
-        <v>0.23689898182666466</v>
-      </c>
-      <c r="L19">
-        <f>_xlfn.STDEV.S(K18:K26)</f>
-        <v>2.4325320751047155</v>
-      </c>
-      <c r="N19">
-        <f>_xlfn.STDEV.S(H9:H16)</f>
-        <v>7.0781383450986704E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F19" s="48">
+        <f>H19*260</f>
+        <v>1.7318343113188992</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" s="7">
+        <f>_xlfn.STDEV.S(H9:H17)</f>
+        <v>6.6609011973803815E-3</v>
+      </c>
+      <c r="I19" s="7">
+        <f>SQRT(_xlfn.VAR.S(I9:I17))</f>
+        <v>1.7318343113188992</v>
+      </c>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="O19" s="7">
+        <f>_xlfn.STDEV.S(O9:O17)</f>
+        <v>6.6594968924920377E-3</v>
+      </c>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="F20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" s="49">
-        <f>G19^(1/COUNT(G9:G16))-1</f>
-        <v>2.186559355780382E-3</v>
-      </c>
-      <c r="H20" s="49">
-        <f>H19^(1/COUNT(L9:L16))-1</f>
-        <v>2.186559355780382E-3</v>
-      </c>
-      <c r="J20" s="17">
-        <f t="shared" si="8"/>
-        <v>0.25890811922203683</v>
-      </c>
-      <c r="K20" s="17">
-        <f t="shared" si="9"/>
-        <v>0.24890811922203682</v>
-      </c>
-      <c r="L20" s="44"/>
-      <c r="N20" s="43">
-        <f>N18/N19</f>
-        <v>0.30858005415466522</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F20" s="6"/>
+      <c r="G20" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="7">
+        <f>SKEW(H9:H17)</f>
+        <v>0.22648502387660699</v>
+      </c>
+      <c r="I20" s="7">
+        <f>SKEW(I9:I17)</f>
+        <v>0.22648502387660754</v>
+      </c>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="50"/>
+      <c r="N20" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="O20" s="7">
+        <f>SKEW(O9:O17)</f>
+        <v>0.22650362677372757</v>
+      </c>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D21" s="5"/>
-      <c r="J21" s="17">
-        <f t="shared" si="8"/>
-        <v>4.6780681872169598</v>
-      </c>
-      <c r="K21" s="17">
-        <f t="shared" si="9"/>
-        <v>4.66806818721696</v>
-      </c>
-      <c r="L21">
-        <f>L18/L19</f>
-        <v>0.28786426408891902</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F21" s="6"/>
+      <c r="G21" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21" s="7">
+        <f>KURT(H9:H17)</f>
+        <v>0.48716396934880812</v>
+      </c>
+      <c r="I21" s="7">
+        <f>KURT(I9:I17)</f>
+        <v>0.48716396934880812</v>
+      </c>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="O21" s="7">
+        <f>KURT(O9:O17)</f>
+        <v>0.48700809395090605</v>
+      </c>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
-      <c r="F22" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" s="4">
-        <f>(AVERAGE(G9:G16)-0.01)/_xlfn.STDEV.S(G9:G16)</f>
-        <v>-1.0980867636013225</v>
-      </c>
-      <c r="J22" s="17">
-        <f t="shared" si="8"/>
-        <v>1.1028474125939736</v>
-      </c>
-      <c r="K22" s="17">
-        <f t="shared" si="9"/>
-        <v>1.0928474125939736</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F22" s="6"/>
+      <c r="G22" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" s="56">
+        <f>H18*260</f>
+        <v>0.50478649031078904</v>
+      </c>
+      <c r="I22" s="48">
+        <f>I18</f>
+        <v>0.50478649031078904</v>
+      </c>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="O22" s="48">
+        <f>O18*260</f>
+        <v>0.50468888888888885</v>
+      </c>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C23" s="22"/>
-      <c r="F23" t="s">
-        <v>56</v>
-      </c>
-      <c r="G23" s="4">
-        <f>(AVERAGE(H9:H16)-0.01)/_xlfn.STDEV.S(H9:H16)*SQRT(365.2422)</f>
-        <v>-21.103107156945686</v>
-      </c>
-      <c r="J23" s="17">
-        <f t="shared" si="8"/>
-        <v>-0.96979844886422917</v>
-      </c>
-      <c r="K23" s="17">
-        <f t="shared" si="9"/>
-        <v>-0.97979844886422918</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J24" s="17">
-        <f t="shared" si="8"/>
-        <v>3.9520068114662004</v>
-      </c>
-      <c r="K24" s="17">
-        <f t="shared" si="9"/>
-        <v>3.9420068114662006</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F25" t="s">
-        <v>46</v>
-      </c>
-      <c r="G25" s="4">
-        <f>(E10-E9)/E9</f>
-        <v>6.7620109268352803E-4</v>
-      </c>
-      <c r="J25" s="17">
-        <f t="shared" si="8"/>
-        <v>0.54700617509859673</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J26" s="17"/>
-      <c r="K26" s="17">
-        <f>J25-0.01</f>
-        <v>0.53700617509859672</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F23" s="6"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F25" s="6"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>39</v>
       </c>
@@ -6836,8 +7033,10 @@
       <c r="F28" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K28" s="56"/>
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>10228</v>
       </c>
@@ -6853,7 +7052,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>10594</v>
       </c>
@@ -6869,7 +7068,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>10959</v>
       </c>
@@ -6882,7 +7081,7 @@
         <v>1100000</v>
       </c>
       <c r="D31">
-        <f t="shared" ref="D31:D41" si="10">G6</f>
+        <f t="shared" ref="D31:D41" si="12">G6</f>
         <v>0</v>
       </c>
       <c r="E31" s="23">
@@ -6890,7 +7089,7 @@
         <v>1100000</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>11324</v>
       </c>
@@ -6903,7 +7102,7 @@
         <v>2100000</v>
       </c>
       <c r="D32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="E32" s="23">
@@ -6922,13 +7121,14 @@
         <f>PRODUCT(G$32:$G32)</f>
         <v>1.9090909090909092</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="17"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>11689</v>
       </c>
       <c r="B33" s="23">
-        <f t="shared" ref="B33:B41" si="11">1000000</f>
+        <f t="shared" ref="B33:B41" si="13">1000000</f>
         <v>1000000</v>
       </c>
       <c r="C33">
@@ -6936,32 +7136,33 @@
         <v>3100000</v>
       </c>
       <c r="D33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="E33" s="23">
-        <f t="shared" ref="E33:E41" si="12">E32*(1+D33)+B33</f>
+        <f t="shared" ref="E33:E41" si="14">E32*(1+D33)+B33</f>
         <v>3100000</v>
       </c>
       <c r="F33" s="21">
-        <f t="shared" ref="F33:F41" si="13">E33/E32-1</f>
+        <f t="shared" ref="F33:F41" si="15">E33/E32-1</f>
         <v>0.47619047619047628</v>
       </c>
       <c r="G33" s="25">
-        <f t="shared" ref="G33:G41" si="14">F33+1</f>
+        <f t="shared" ref="G33:G41" si="16">F33+1</f>
         <v>1.4761904761904763</v>
       </c>
       <c r="H33" s="17">
         <f>PRODUCT(G$32:$G33)</f>
         <v>2.8181818181818183</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="17"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>12055</v>
       </c>
       <c r="B34" s="23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="C34">
@@ -6969,32 +7170,33 @@
         <v>4100000</v>
       </c>
       <c r="D34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-9.357139928022673E-3</v>
       </c>
       <c r="E34" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>4070992.8662231299</v>
       </c>
       <c r="F34" s="21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.3132235052332677</v>
       </c>
       <c r="G34" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.3132235052332677</v>
       </c>
       <c r="H34" s="17">
         <f>PRODUCT(G$32:$G34)</f>
         <v>3.700902605657391</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="17"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>12420</v>
       </c>
       <c r="B35" s="23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="C35">
@@ -7002,32 +7204,33 @@
         <v>5100000</v>
       </c>
       <c r="D35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>6.7620109268351491E-4</v>
       </c>
       <c r="E35" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>5073745.6760475766</v>
       </c>
       <c r="F35" s="21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.24631652345653765</v>
       </c>
       <c r="G35" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.2463165234565377</v>
       </c>
       <c r="H35" s="17">
         <f>PRODUCT(G$32:$G35)</f>
         <v>4.6124960691341608</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="17"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>12785</v>
       </c>
       <c r="B36" s="23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="C36">
@@ -7035,32 +7238,33 @@
         <v>6100000</v>
       </c>
       <c r="D36">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>7.0910309281613237E-4</v>
       </c>
       <c r="E36" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>6077343.4847986242</v>
       </c>
       <c r="F36" s="21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.19780215107920918</v>
       </c>
       <c r="G36" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.1978021510792092</v>
       </c>
       <c r="H36" s="17">
         <f>PRODUCT(G$32:$G36)</f>
         <v>5.5248577134532946</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="17"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>13150</v>
       </c>
       <c r="B37" s="23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="C37">
@@ -7068,32 +7272,33 @@
         <v>7100000</v>
       </c>
       <c r="D37">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.2890224506745485E-2</v>
       </c>
       <c r="E37" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>7155681.8067222852</v>
       </c>
       <c r="F37" s="21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.17743580309734508</v>
       </c>
       <c r="G37" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.1774358030973451</v>
       </c>
       <c r="H37" s="17">
         <f>PRODUCT(G$32:$G37)</f>
         <v>6.5051652788384411</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="17"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>13516</v>
       </c>
       <c r="B38" s="23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="C38">
@@ -7101,32 +7306,33 @@
         <v>8100000</v>
       </c>
       <c r="D38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>3.0239947318970728E-3</v>
       </c>
       <c r="E38" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8177320.5508089447</v>
       </c>
       <c r="F38" s="21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.14277308182246151</v>
       </c>
       <c r="G38" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.1427730818224615</v>
       </c>
       <c r="H38" s="17">
         <f>PRODUCT(G$32:$G38)</f>
         <v>7.4339277734626776</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="17"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>13881</v>
       </c>
       <c r="B39" s="23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="C39">
@@ -7134,32 +7340,33 @@
         <v>9100000</v>
       </c>
       <c r="D39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-2.6516416178182789E-3</v>
       </c>
       <c r="E39" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>9155637.2273141779</v>
       </c>
       <c r="F39" s="21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.11963780439161731</v>
       </c>
       <c r="G39" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.1196378043916173</v>
       </c>
       <c r="H39" s="17">
         <f>PRODUCT(G$32:$G39)</f>
         <v>8.3233065702856166</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="17"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>14246</v>
       </c>
       <c r="B40" s="23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="C40">
@@ -7167,32 +7374,33 @@
         <v>10100000</v>
       </c>
       <c r="D40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.0878752906358091E-2</v>
       </c>
       <c r="E40" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>10255239.142410383</v>
       </c>
       <c r="F40" s="21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.12010107956393723</v>
       </c>
       <c r="G40" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.1201010795639372</v>
       </c>
       <c r="H40" s="17">
         <f>PRODUCT(G$32:$G40)</f>
         <v>9.3229446749185314</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="17"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>14611</v>
       </c>
       <c r="B41" s="23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="C41">
@@ -7200,35 +7408,36 @@
         <v>11100000</v>
       </c>
       <c r="D41">
-        <f t="shared" si="10"/>
+        <f>G17</f>
         <v>1.4987432818573954E-3</v>
       </c>
       <c r="E41" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>11270609.113178911</v>
       </c>
       <c r="F41" s="21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>9.9009877455658923E-2</v>
       </c>
       <c r="G41" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0990098774556589</v>
       </c>
       <c r="H41" s="17">
         <f>PRODUCT(G$32:$G41)</f>
         <v>10.246008284708104</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="17"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E42" s="24"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
         <v>34</v>
       </c>
@@ -7238,7 +7447,7 @@
       </c>
       <c r="G44" s="20"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
         <v>33</v>
       </c>
@@ -7248,7 +7457,7 @@
       </c>
       <c r="G45" s="3"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
         <v>35</v>
       </c>
@@ -7257,7 +7466,7 @@
         <v>1.0534636927554566</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E48" t="s">
         <v>36</v>
       </c>

</xml_diff>